<commit_message>
Standardize all solutions on credit-based cost format
- Rewrote compute-costs.py to support credit-based format only
- Converted solution-template to 9-column credit format with generic content
- Fixed Azure document-intelligence architecture diagram embedding
- Updated document-intelligence LOE with correct IDP tasks
- Updated COST_CREDITS_GUIDANCE.md to reflect credit-based as standard
- Fixed logo paths in solution-template PowerPoint
- Regenerated all Word, PowerPoint, and Excel outputs
</commit_message>
<xml_diff>
--- a/solutions/azure/ai/document-intelligence/presales/level-of-effort-estimate.xlsx
+++ b/solutions/azure/ai/document-intelligence/presales/level-of-effort-estimate.xlsx
@@ -21,7 +21,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="$#,##0"/>
+  </numFmts>
   <fonts count="9">
     <font>
       <name val="Calibri"/>
@@ -75,7 +77,7 @@
       <sz val="12"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -100,6 +102,18 @@
         <bgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF2CC"/>
+        <bgColor rgb="00FFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E8F4F8"/>
+        <bgColor rgb="00E8F4F8"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -119,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
@@ -142,6 +156,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -580,7 +612,7 @@
       </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
-          <t>November 13, 2025</t>
+          <t>November 15, 2025</t>
         </is>
       </c>
     </row>
@@ -637,7 +669,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -657,34 +689,645 @@
     <row r="1" ht="32" customHeight="1">
       <c r="A1" s="5" t="inlineStr">
         <is>
-          <t>Column 1</t>
+          <t>Category</t>
         </is>
       </c>
       <c r="B1" s="5" t="inlineStr">
         <is>
-          <t>Column 2</t>
+          <t>Baseline Assumption</t>
         </is>
       </c>
       <c r="C1" s="5" t="inlineStr">
         <is>
-          <t>Column 3</t>
+          <t>Small (1x)</t>
         </is>
       </c>
       <c r="D1" s="5" t="inlineStr">
         <is>
-          <t>Column 4</t>
+          <t>Medium (2x)</t>
         </is>
       </c>
       <c r="E1" s="5" t="inlineStr">
         <is>
-          <t>Column 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" ht="26" customHeight="1"/>
-    <row r="3" ht="26" customHeight="1"/>
-    <row r="4" ht="26" customHeight="1"/>
-    <row r="5" ht="26" customHeight="1"/>
+          <t>Large (3x)</t>
+        </is>
+      </c>
+      <c r="F1" s="5" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="G1" s="5" t="inlineStr"/>
+      <c r="H1" s="5" t="inlineStr"/>
+      <c r="I1" s="5" t="inlineStr"/>
+      <c r="J1" s="5" t="inlineStr"/>
+      <c r="K1" s="5" t="inlineStr"/>
+    </row>
+    <row r="2" ht="26" customHeight="1">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>Solution Scope</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="inlineStr">
+        <is>
+          <t>Document Types</t>
+        </is>
+      </c>
+      <c r="C2" s="6" t="inlineStr">
+        <is>
+          <t>2-3 document types</t>
+        </is>
+      </c>
+      <c r="D2" s="6" t="inlineStr">
+        <is>
+          <t>4-6 document types</t>
+        </is>
+      </c>
+      <c r="E2" s="6" t="inlineStr">
+        <is>
+          <t>8+ document types or complex variations</t>
+        </is>
+      </c>
+      <c r="F2" s="6" t="inlineStr">
+        <is>
+          <t>Standard document types for IDP</t>
+        </is>
+      </c>
+      <c r="G2" s="6" t="inlineStr"/>
+      <c r="H2" s="6" t="inlineStr"/>
+      <c r="I2" s="6" t="inlineStr"/>
+      <c r="J2" s="6" t="inlineStr"/>
+      <c r="K2" s="6" t="inlineStr"/>
+    </row>
+    <row r="3" ht="26" customHeight="1">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>Solution Scope</t>
+        </is>
+      </c>
+      <c r="B3" s="7" t="inlineStr">
+        <is>
+          <t>AI/ML Complexity</t>
+        </is>
+      </c>
+      <c r="C3" s="7" t="inlineStr">
+        <is>
+          <t>Azure Document Intelligence only</t>
+        </is>
+      </c>
+      <c r="D3" s="7" t="inlineStr">
+        <is>
+          <t>Custom classification models</t>
+        </is>
+      </c>
+      <c r="E3" s="7" t="inlineStr">
+        <is>
+          <t>Advanced custom models + NLP</t>
+        </is>
+      </c>
+      <c r="F3" s="7" t="inlineStr">
+        <is>
+          <t>Pre-built vs custom model development</t>
+        </is>
+      </c>
+      <c r="G3" s="7" t="inlineStr"/>
+      <c r="H3" s="7" t="inlineStr"/>
+      <c r="I3" s="7" t="inlineStr"/>
+      <c r="J3" s="7" t="inlineStr"/>
+      <c r="K3" s="7" t="inlineStr"/>
+    </row>
+    <row r="4" ht="26" customHeight="1">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>Integration</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>External System Integrations</t>
+        </is>
+      </c>
+      <c r="C4" s="6" t="inlineStr">
+        <is>
+          <t>2 REST APIs</t>
+        </is>
+      </c>
+      <c r="D4" s="6" t="inlineStr">
+        <is>
+          <t>4-6 systems</t>
+        </is>
+      </c>
+      <c r="E4" s="6" t="inlineStr">
+        <is>
+          <t>8+ systems or complex protocols</t>
+        </is>
+      </c>
+      <c r="F4" s="6" t="inlineStr">
+        <is>
+          <t>Standard REST/API integrations for document flow</t>
+        </is>
+      </c>
+      <c r="G4" s="6" t="inlineStr"/>
+      <c r="H4" s="6" t="inlineStr"/>
+      <c r="I4" s="6" t="inlineStr"/>
+      <c r="J4" s="6" t="inlineStr"/>
+      <c r="K4" s="6" t="inlineStr"/>
+    </row>
+    <row r="5" ht="26" customHeight="1">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>Integration</t>
+        </is>
+      </c>
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>Data Sources</t>
+        </is>
+      </c>
+      <c r="C5" s="7" t="inlineStr">
+        <is>
+          <t>2-3 data sources</t>
+        </is>
+      </c>
+      <c r="D5" s="7" t="inlineStr">
+        <is>
+          <t>4-6 data sources</t>
+        </is>
+      </c>
+      <c r="E5" s="7" t="inlineStr">
+        <is>
+          <t>8+ data sources or complex formats</t>
+        </is>
+      </c>
+      <c r="F5" s="7" t="inlineStr">
+        <is>
+          <t>Document input channels and storage</t>
+        </is>
+      </c>
+      <c r="G5" s="7" t="inlineStr"/>
+      <c r="H5" s="7" t="inlineStr"/>
+      <c r="I5" s="7" t="inlineStr"/>
+      <c r="J5" s="7" t="inlineStr"/>
+      <c r="K5" s="7" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="inlineStr">
+        <is>
+          <t>User Base</t>
+        </is>
+      </c>
+      <c r="B6" s="6" t="inlineStr">
+        <is>
+          <t>Total Users</t>
+        </is>
+      </c>
+      <c r="C6" s="6" t="inlineStr">
+        <is>
+          <t>50 users</t>
+        </is>
+      </c>
+      <c r="D6" s="6" t="inlineStr">
+        <is>
+          <t>100-250 users</t>
+        </is>
+      </c>
+      <c r="E6" s="6" t="inlineStr">
+        <is>
+          <t>500+ users</t>
+        </is>
+      </c>
+      <c r="F6" s="6" t="inlineStr">
+        <is>
+          <t>Users submitting and reviewing documents</t>
+        </is>
+      </c>
+      <c r="G6" s="6" t="inlineStr"/>
+      <c r="H6" s="6" t="inlineStr"/>
+      <c r="I6" s="6" t="inlineStr"/>
+      <c r="J6" s="6" t="inlineStr"/>
+      <c r="K6" s="6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="inlineStr">
+        <is>
+          <t>User Base</t>
+        </is>
+      </c>
+      <c r="B7" s="7" t="inlineStr">
+        <is>
+          <t>User Roles</t>
+        </is>
+      </c>
+      <c r="C7" s="7" t="inlineStr">
+        <is>
+          <t>2-3 standard roles</t>
+        </is>
+      </c>
+      <c r="D7" s="7" t="inlineStr">
+        <is>
+          <t>4-6 roles</t>
+        </is>
+      </c>
+      <c r="E7" s="7" t="inlineStr">
+        <is>
+          <t>8+ roles with complex permissions</t>
+        </is>
+      </c>
+      <c r="F7" s="7" t="inlineStr">
+        <is>
+          <t>Document processors reviewers administrators</t>
+        </is>
+      </c>
+      <c r="G7" s="7" t="inlineStr"/>
+      <c r="H7" s="7" t="inlineStr"/>
+      <c r="I7" s="7" t="inlineStr"/>
+      <c r="J7" s="7" t="inlineStr"/>
+      <c r="K7" s="7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="inlineStr">
+        <is>
+          <t>Data Volume</t>
+        </is>
+      </c>
+      <c r="B8" s="6" t="inlineStr">
+        <is>
+          <t>Document Processing Volume</t>
+        </is>
+      </c>
+      <c r="C8" s="6" t="inlineStr">
+        <is>
+          <t>1000-5000 docs/month</t>
+        </is>
+      </c>
+      <c r="D8" s="6" t="inlineStr">
+        <is>
+          <t>10000-50000 docs/month</t>
+        </is>
+      </c>
+      <c r="E8" s="6" t="inlineStr">
+        <is>
+          <t>100000+ docs/month</t>
+        </is>
+      </c>
+      <c r="F8" s="6" t="inlineStr">
+        <is>
+          <t>Monthly document processing volume</t>
+        </is>
+      </c>
+      <c r="G8" s="6" t="inlineStr"/>
+      <c r="H8" s="6" t="inlineStr"/>
+      <c r="I8" s="6" t="inlineStr"/>
+      <c r="J8" s="6" t="inlineStr"/>
+      <c r="K8" s="6" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>Data Volume</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>Data Storage Requirements</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="inlineStr">
+        <is>
+          <t>500 GB</t>
+        </is>
+      </c>
+      <c r="D9" s="7" t="inlineStr">
+        <is>
+          <t>2 TB</t>
+        </is>
+      </c>
+      <c r="E9" s="7" t="inlineStr">
+        <is>
+          <t>10+ TB</t>
+        </is>
+      </c>
+      <c r="F9" s="7" t="inlineStr">
+        <is>
+          <t>Document storage and retention</t>
+        </is>
+      </c>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="7" t="inlineStr"/>
+      <c r="I9" s="7" t="inlineStr"/>
+      <c r="J9" s="7" t="inlineStr"/>
+      <c r="K9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>Technical Environment</t>
+        </is>
+      </c>
+      <c r="B10" s="6" t="inlineStr">
+        <is>
+          <t>Deployment Regions</t>
+        </is>
+      </c>
+      <c r="C10" s="6" t="inlineStr">
+        <is>
+          <t>Single Azure region</t>
+        </is>
+      </c>
+      <c r="D10" s="6" t="inlineStr">
+        <is>
+          <t>2-3 regions</t>
+        </is>
+      </c>
+      <c r="E10" s="6" t="inlineStr">
+        <is>
+          <t>Global multi-region</t>
+        </is>
+      </c>
+      <c r="F10" s="6" t="inlineStr">
+        <is>
+          <t>Geographic distribution for IDP</t>
+        </is>
+      </c>
+      <c r="G10" s="6" t="inlineStr"/>
+      <c r="H10" s="6" t="inlineStr"/>
+      <c r="I10" s="6" t="inlineStr"/>
+      <c r="J10" s="6" t="inlineStr"/>
+      <c r="K10" s="6" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>Technical Environment</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>Availability Requirements</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="inlineStr">
+        <is>
+          <t>Standard (99.5%)</t>
+        </is>
+      </c>
+      <c r="D11" s="7" t="inlineStr">
+        <is>
+          <t>High availability (99.9%)</t>
+        </is>
+      </c>
+      <c r="E11" s="7" t="inlineStr">
+        <is>
+          <t>Mission critical (99.95%+)</t>
+        </is>
+      </c>
+      <c r="F11" s="7" t="inlineStr">
+        <is>
+          <t>SLA for document processing</t>
+        </is>
+      </c>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+      <c r="I11" s="7" t="inlineStr"/>
+      <c r="J11" s="7" t="inlineStr"/>
+      <c r="K11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>Technical Environment</t>
+        </is>
+      </c>
+      <c r="B12" s="6" t="inlineStr">
+        <is>
+          <t>Infrastructure Complexity</t>
+        </is>
+      </c>
+      <c r="C12" s="6" t="inlineStr">
+        <is>
+          <t>Basic serverless</t>
+        </is>
+      </c>
+      <c r="D12" s="6" t="inlineStr">
+        <is>
+          <t>Multi-tier standard</t>
+        </is>
+      </c>
+      <c r="E12" s="6" t="inlineStr">
+        <is>
+          <t>Complex distributed with custom ML</t>
+        </is>
+      </c>
+      <c r="F12" s="6" t="inlineStr">
+        <is>
+          <t>Azure Functions Blob Storage Document Intelligence architecture</t>
+        </is>
+      </c>
+      <c r="G12" s="6" t="inlineStr"/>
+      <c r="H12" s="6" t="inlineStr"/>
+      <c r="I12" s="6" t="inlineStr"/>
+      <c r="J12" s="6" t="inlineStr"/>
+      <c r="K12" s="6" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="inlineStr">
+        <is>
+          <t>Security &amp; Compliance</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>Security Requirements</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr">
+        <is>
+          <t>Basic encryption RBAC</t>
+        </is>
+      </c>
+      <c r="D13" s="7" t="inlineStr">
+        <is>
+          <t>Industry standard (SOC2 HIPAA)</t>
+        </is>
+      </c>
+      <c r="E13" s="7" t="inlineStr">
+        <is>
+          <t>Advanced (FedRAMP multi-jurisdiction)</t>
+        </is>
+      </c>
+      <c r="F13" s="7" t="inlineStr">
+        <is>
+          <t>Document security and access controls</t>
+        </is>
+      </c>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="7" t="inlineStr"/>
+      <c r="I13" s="7" t="inlineStr"/>
+      <c r="J13" s="7" t="inlineStr"/>
+      <c r="K13" s="7" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="inlineStr">
+        <is>
+          <t>Security &amp; Compliance</t>
+        </is>
+      </c>
+      <c r="B14" s="6" t="inlineStr">
+        <is>
+          <t>Compliance Frameworks</t>
+        </is>
+      </c>
+      <c r="C14" s="6" t="inlineStr">
+        <is>
+          <t>1-2 basic standards</t>
+        </is>
+      </c>
+      <c r="D14" s="6" t="inlineStr">
+        <is>
+          <t>2-3 industry standards</t>
+        </is>
+      </c>
+      <c r="E14" s="6" t="inlineStr">
+        <is>
+          <t>Multiple complex frameworks</t>
+        </is>
+      </c>
+      <c r="F14" s="6" t="inlineStr">
+        <is>
+          <t>Regulatory compliance for documents</t>
+        </is>
+      </c>
+      <c r="G14" s="6" t="inlineStr"/>
+      <c r="H14" s="6" t="inlineStr"/>
+      <c r="I14" s="6" t="inlineStr"/>
+      <c r="J14" s="6" t="inlineStr"/>
+      <c r="K14" s="6" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="inlineStr">
+        <is>
+          <t>Performance</t>
+        </is>
+      </c>
+      <c r="B15" s="7" t="inlineStr">
+        <is>
+          <t>Accuracy Requirements</t>
+        </is>
+      </c>
+      <c r="C15" s="7" t="inlineStr">
+        <is>
+          <t>95%+ standard</t>
+        </is>
+      </c>
+      <c r="D15" s="7" t="inlineStr">
+        <is>
+          <t>98%+ enhanced</t>
+        </is>
+      </c>
+      <c r="E15" s="7" t="inlineStr">
+        <is>
+          <t>99%+ with human review</t>
+        </is>
+      </c>
+      <c r="F15" s="7" t="inlineStr">
+        <is>
+          <t>Data extraction accuracy targets</t>
+        </is>
+      </c>
+      <c r="G15" s="7" t="inlineStr"/>
+      <c r="H15" s="7" t="inlineStr"/>
+      <c r="I15" s="7" t="inlineStr"/>
+      <c r="J15" s="7" t="inlineStr"/>
+      <c r="K15" s="7" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="inlineStr">
+        <is>
+          <t>Performance</t>
+        </is>
+      </c>
+      <c r="B16" s="6" t="inlineStr">
+        <is>
+          <t>Processing Speed</t>
+        </is>
+      </c>
+      <c r="C16" s="6" t="inlineStr">
+        <is>
+          <t>Standard batch processing</t>
+        </is>
+      </c>
+      <c r="D16" s="6" t="inlineStr">
+        <is>
+          <t>Near real-time processing</t>
+        </is>
+      </c>
+      <c r="E16" s="6" t="inlineStr">
+        <is>
+          <t>Real-time with sub-second response</t>
+        </is>
+      </c>
+      <c r="F16" s="6" t="inlineStr">
+        <is>
+          <t>Document processing speed requirements</t>
+        </is>
+      </c>
+      <c r="G16" s="6" t="inlineStr"/>
+      <c r="H16" s="6" t="inlineStr"/>
+      <c r="I16" s="6" t="inlineStr"/>
+      <c r="J16" s="6" t="inlineStr"/>
+      <c r="K16" s="6" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="inlineStr">
+        <is>
+          <t>Environment</t>
+        </is>
+      </c>
+      <c r="B17" s="7" t="inlineStr">
+        <is>
+          <t>Deployment Environments</t>
+        </is>
+      </c>
+      <c r="C17" s="7" t="inlineStr">
+        <is>
+          <t>2 environments (dev prod)</t>
+        </is>
+      </c>
+      <c r="D17" s="7" t="inlineStr">
+        <is>
+          <t>3 environments (dev staging prod)</t>
+        </is>
+      </c>
+      <c r="E17" s="7" t="inlineStr">
+        <is>
+          <t>4+ environments with ML pipelines</t>
+        </is>
+      </c>
+      <c r="F17" s="7" t="inlineStr">
+        <is>
+          <t>Environment management for IDP</t>
+        </is>
+      </c>
+      <c r="G17" s="7" t="inlineStr"/>
+      <c r="H17" s="7" t="inlineStr"/>
+      <c r="I17" s="7" t="inlineStr"/>
+      <c r="J17" s="7" t="inlineStr"/>
+      <c r="K17" s="7" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="inlineStr"/>
+      <c r="B18" s="6" t="inlineStr"/>
+      <c r="C18" s="6" t="inlineStr"/>
+      <c r="D18" s="6" t="inlineStr"/>
+      <c r="E18" s="6" t="inlineStr"/>
+      <c r="F18" s="6" t="inlineStr"/>
+      <c r="G18" s="6" t="inlineStr"/>
+      <c r="H18" s="6" t="inlineStr"/>
+      <c r="I18" s="6" t="inlineStr"/>
+      <c r="J18" s="6" t="inlineStr"/>
+      <c r="K18" s="6" t="inlineStr"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -697,7 +1340,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -845,7 +1488,291 @@
         </is>
       </c>
     </row>
-    <row r="23" ht="32" customHeight="1"/>
+    <row r="23" ht="32" customHeight="1">
+      <c r="A23" s="5" t="inlineStr">
+        <is>
+          <t>Phase</t>
+        </is>
+      </c>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>Variable Name</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>Multiplier</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="inlineStr">
+        <is>
+          <t>Description / Applies To Tasks</t>
+        </is>
+      </c>
+      <c r="E23" s="5" t="inlineStr"/>
+      <c r="F23" s="5" t="inlineStr"/>
+      <c r="G23" s="5" t="inlineStr"/>
+      <c r="H23" s="5" t="inlineStr"/>
+      <c r="I23" s="5" t="inlineStr"/>
+      <c r="J23" s="5" t="inlineStr"/>
+      <c r="K23" s="5" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="inlineStr">
+        <is>
+          <t>Discovery</t>
+        </is>
+      </c>
+      <c r="B24" s="6" t="inlineStr">
+        <is>
+          <t>DISCOVERY_MX</t>
+        </is>
+      </c>
+      <c r="C24" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="6" t="inlineStr">
+        <is>
+          <t>All Discovery phase tasks (Requirements Gathering, Document Analysis, Azure Assessment, Compliance Review)</t>
+        </is>
+      </c>
+      <c r="E24" s="6" t="inlineStr"/>
+      <c r="F24" s="6" t="inlineStr"/>
+      <c r="G24" s="6" t="inlineStr"/>
+      <c r="H24" s="6" t="inlineStr"/>
+      <c r="I24" s="6" t="inlineStr"/>
+      <c r="J24" s="6" t="inlineStr"/>
+      <c r="K24" s="6" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="7" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="B25" s="7" t="inlineStr">
+        <is>
+          <t>PLANNING_MX</t>
+        </is>
+      </c>
+      <c r="C25" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="7" t="inlineStr">
+        <is>
+          <t>All Planning phase tasks (IDP Solution Design, Data Flow Design, Security Architecture, Project Planning)</t>
+        </is>
+      </c>
+      <c r="E25" s="7" t="inlineStr"/>
+      <c r="F25" s="7" t="inlineStr"/>
+      <c r="G25" s="7" t="inlineStr"/>
+      <c r="H25" s="7" t="inlineStr"/>
+      <c r="I25" s="7" t="inlineStr"/>
+      <c r="J25" s="7" t="inlineStr"/>
+      <c r="K25" s="7" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="inlineStr">
+        <is>
+          <t>Development</t>
+        </is>
+      </c>
+      <c r="B26" s="6" t="inlineStr">
+        <is>
+          <t>DEVELOPMENT_MX</t>
+        </is>
+      </c>
+      <c r="C26" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" s="6" t="inlineStr">
+        <is>
+          <t>All Development phase tasks (Azure Infrastructure, Document Pipeline, AI/ML Integration, Custom Models, API Development)</t>
+        </is>
+      </c>
+      <c r="E26" s="6" t="inlineStr"/>
+      <c r="F26" s="6" t="inlineStr"/>
+      <c r="G26" s="6" t="inlineStr"/>
+      <c r="H26" s="6" t="inlineStr"/>
+      <c r="I26" s="6" t="inlineStr"/>
+      <c r="J26" s="6" t="inlineStr"/>
+      <c r="K26" s="6" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="7" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+      <c r="B27" s="7" t="inlineStr">
+        <is>
+          <t>TESTING_MX</t>
+        </is>
+      </c>
+      <c r="C27" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="7" t="inlineStr">
+        <is>
+          <t>All Testing phase tasks (Unit Testing, Document Testing, Performance Testing, Accuracy Testing, Security Testing)</t>
+        </is>
+      </c>
+      <c r="E27" s="7" t="inlineStr"/>
+      <c r="F27" s="7" t="inlineStr"/>
+      <c r="G27" s="7" t="inlineStr"/>
+      <c r="H27" s="7" t="inlineStr"/>
+      <c r="I27" s="7" t="inlineStr"/>
+      <c r="J27" s="7" t="inlineStr"/>
+      <c r="K27" s="7" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="inlineStr">
+        <is>
+          <t>Deployment</t>
+        </is>
+      </c>
+      <c r="B28" s="6" t="inlineStr">
+        <is>
+          <t>DEPLOYMENT_MX</t>
+        </is>
+      </c>
+      <c r="C28" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="6" t="inlineStr">
+        <is>
+          <t>All Deployment phase tasks (Production Deployment, Model Deployment, Go-Live Support)</t>
+        </is>
+      </c>
+      <c r="E28" s="6" t="inlineStr"/>
+      <c r="F28" s="6" t="inlineStr"/>
+      <c r="G28" s="6" t="inlineStr"/>
+      <c r="H28" s="6" t="inlineStr"/>
+      <c r="I28" s="6" t="inlineStr"/>
+      <c r="J28" s="6" t="inlineStr"/>
+      <c r="K28" s="6" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="7" t="inlineStr">
+        <is>
+          <t>Training</t>
+        </is>
+      </c>
+      <c r="B29" s="7" t="inlineStr">
+        <is>
+          <t>TRAINING_MX</t>
+        </is>
+      </c>
+      <c r="C29" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="7" t="inlineStr">
+        <is>
+          <t>All Training phase tasks (Administrator Training, Business User Training, Documentation)</t>
+        </is>
+      </c>
+      <c r="E29" s="7" t="inlineStr"/>
+      <c r="F29" s="7" t="inlineStr"/>
+      <c r="G29" s="7" t="inlineStr"/>
+      <c r="H29" s="7" t="inlineStr"/>
+      <c r="I29" s="7" t="inlineStr"/>
+      <c r="J29" s="7" t="inlineStr"/>
+      <c r="K29" s="7" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="inlineStr">
+        <is>
+          <t>Closeout</t>
+        </is>
+      </c>
+      <c r="B30" s="6" t="inlineStr">
+        <is>
+          <t>CLOSEOUT_MX</t>
+        </is>
+      </c>
+      <c r="C30" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="6" t="inlineStr">
+        <is>
+          <t>All Closeout phase tasks (Knowledge Transfer, Performance Baseline)</t>
+        </is>
+      </c>
+      <c r="E30" s="6" t="inlineStr"/>
+      <c r="F30" s="6" t="inlineStr"/>
+      <c r="G30" s="6" t="inlineStr"/>
+      <c r="H30" s="6" t="inlineStr"/>
+      <c r="I30" s="6" t="inlineStr"/>
+      <c r="J30" s="6" t="inlineStr"/>
+      <c r="K30" s="6" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="7" t="inlineStr">
+        <is>
+          <t>Management</t>
+        </is>
+      </c>
+      <c r="B31" s="7" t="inlineStr">
+        <is>
+          <t>MANAGEMENT_MX</t>
+        </is>
+      </c>
+      <c r="C31" s="12" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="D31" s="7" t="inlineStr">
+        <is>
+          <t>Project Management overhead - 10% of actual engineering hours</t>
+        </is>
+      </c>
+      <c r="E31" s="7" t="inlineStr"/>
+      <c r="F31" s="7" t="inlineStr"/>
+      <c r="G31" s="7" t="inlineStr"/>
+      <c r="H31" s="7" t="inlineStr"/>
+      <c r="I31" s="7" t="inlineStr"/>
+      <c r="J31" s="7" t="inlineStr"/>
+      <c r="K31" s="7" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="6" t="inlineStr">
+        <is>
+          <t>Leadership</t>
+        </is>
+      </c>
+      <c r="B32" s="6" t="inlineStr">
+        <is>
+          <t>LEADERSHIP_MX</t>
+        </is>
+      </c>
+      <c r="C32" s="12" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="D32" s="6" t="inlineStr">
+        <is>
+          <t>Quarterback/Technical Leadership overhead - 10% of actual engineering hours</t>
+        </is>
+      </c>
+      <c r="E32" s="6" t="inlineStr"/>
+      <c r="F32" s="6" t="inlineStr"/>
+      <c r="G32" s="6" t="inlineStr"/>
+      <c r="H32" s="6" t="inlineStr"/>
+      <c r="I32" s="6" t="inlineStr"/>
+      <c r="J32" s="6" t="inlineStr"/>
+      <c r="K32" s="6" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="7" t="inlineStr"/>
+      <c r="B33" s="7" t="inlineStr"/>
+      <c r="C33" s="12" t="inlineStr"/>
+      <c r="D33" s="7" t="inlineStr"/>
+      <c r="E33" s="7" t="inlineStr"/>
+      <c r="F33" s="7" t="inlineStr"/>
+      <c r="G33" s="7" t="inlineStr"/>
+      <c r="H33" s="7" t="inlineStr"/>
+      <c r="I33" s="7" t="inlineStr"/>
+      <c r="J33" s="7" t="inlineStr"/>
+      <c r="K33" s="7" t="inlineStr"/>
+    </row>
   </sheetData>
   <mergeCells count="17">
     <mergeCell ref="A1:D1"/>
@@ -876,7 +1803,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -898,7 +1825,1572 @@
     <col width="60" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
-    <row r="1" ht="32" customHeight="1"/>
+    <row r="1" ht="32" customHeight="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>Phase</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>Work Package</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>Task Description</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>Resource Type</t>
+        </is>
+      </c>
+      <c r="E1" s="5" t="inlineStr">
+        <is>
+          <t>Base Hours</t>
+        </is>
+      </c>
+      <c r="F1" s="5" t="inlineStr">
+        <is>
+          <t>Effort Multiplier</t>
+        </is>
+      </c>
+      <c r="G1" s="5" t="inlineStr">
+        <is>
+          <t>Actual Hours</t>
+        </is>
+      </c>
+      <c r="H1" s="5" t="inlineStr">
+        <is>
+          <t>Rate</t>
+        </is>
+      </c>
+      <c r="I1" s="5" t="inlineStr">
+        <is>
+          <t>Cost Estimate</t>
+        </is>
+      </c>
+      <c r="J1" s="5" t="inlineStr">
+        <is>
+          <t>Dependencies</t>
+        </is>
+      </c>
+      <c r="K1" s="5" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>Discovery</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="inlineStr">
+        <is>
+          <t>Requirements Gathering</t>
+        </is>
+      </c>
+      <c r="C2" s="6" t="inlineStr">
+        <is>
+          <t>Conduct stakeholder interviews for IDP requirements</t>
+        </is>
+      </c>
+      <c r="D2" s="6" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E2" s="13" t="n">
+        <v>32</v>
+      </c>
+      <c r="F2" s="14">
+        <f>'Estimate Settings'!$C$24</f>
+        <v/>
+      </c>
+      <c r="G2" s="6">
+        <f>$E2*$F2</f>
+        <v/>
+      </c>
+      <c r="H2" s="15" t="n">
+        <v>150</v>
+      </c>
+      <c r="I2" s="6">
+        <f>TEXT($G2*$H2,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J2" s="6" t="inlineStr"/>
+      <c r="K2" s="6" t="inlineStr">
+        <is>
+          <t>Includes requirements documentation and document processing workflow analysis</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>Discovery</t>
+        </is>
+      </c>
+      <c r="B3" s="7" t="inlineStr">
+        <is>
+          <t>Document Analysis</t>
+        </is>
+      </c>
+      <c r="C3" s="7" t="inlineStr">
+        <is>
+          <t>Analyze document types volumes and data extraction requirements</t>
+        </is>
+      </c>
+      <c r="D3" s="7" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E3" s="16" t="n">
+        <v>24</v>
+      </c>
+      <c r="F3" s="14">
+        <f>'Estimate Settings'!$C$24</f>
+        <v/>
+      </c>
+      <c r="G3" s="7">
+        <f>$E3*$F3</f>
+        <v/>
+      </c>
+      <c r="H3" s="17" t="n">
+        <v>200</v>
+      </c>
+      <c r="I3" s="7">
+        <f>TEXT($G3*$H3,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J3" s="7" t="inlineStr"/>
+      <c r="K3" s="7" t="inlineStr">
+        <is>
+          <t>Customer must provide representative document samples for each document type</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>Discovery</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>Azure Environment Assessment</t>
+        </is>
+      </c>
+      <c r="C4" s="6" t="inlineStr">
+        <is>
+          <t>Evaluate Azure infrastructure and AI/ML services readiness</t>
+        </is>
+      </c>
+      <c r="D4" s="6" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E4" s="13" t="n">
+        <v>24</v>
+      </c>
+      <c r="F4" s="14">
+        <f>'Estimate Settings'!$C$24</f>
+        <v/>
+      </c>
+      <c r="G4" s="6">
+        <f>$E4*$F4</f>
+        <v/>
+      </c>
+      <c r="H4" s="15" t="n">
+        <v>200</v>
+      </c>
+      <c r="I4" s="6">
+        <f>TEXT($G4*$H4,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J4" s="6" t="inlineStr"/>
+      <c r="K4" s="6" t="inlineStr">
+        <is>
+          <t>Customer must provide Azure subscription access and service limits information</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>Discovery</t>
+        </is>
+      </c>
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>Compliance Review</t>
+        </is>
+      </c>
+      <c r="C5" s="7" t="inlineStr">
+        <is>
+          <t>Assess data privacy compliance and security requirements</t>
+        </is>
+      </c>
+      <c r="D5" s="7" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E5" s="16" t="n">
+        <v>16</v>
+      </c>
+      <c r="F5" s="14">
+        <f>'Estimate Settings'!$C$24</f>
+        <v/>
+      </c>
+      <c r="G5" s="7">
+        <f>$E5*$F5</f>
+        <v/>
+      </c>
+      <c r="H5" s="17" t="n">
+        <v>175</v>
+      </c>
+      <c r="I5" s="7">
+        <f>TEXT($G5*$H5,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J5" s="7" t="inlineStr"/>
+      <c r="K5" s="7" t="inlineStr">
+        <is>
+          <t>Identifies PII/PHI handling requirements and document retention policies</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="B6" s="6" t="inlineStr">
+        <is>
+          <t>IDP Solution Design</t>
+        </is>
+      </c>
+      <c r="C6" s="6" t="inlineStr">
+        <is>
+          <t>Design Azure AI/ML architecture with Document Intelligence and Cognitive Services</t>
+        </is>
+      </c>
+      <c r="D6" s="6" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E6" s="13" t="n">
+        <v>40</v>
+      </c>
+      <c r="F6" s="14">
+        <f>'Estimate Settings'!$C$25</f>
+        <v/>
+      </c>
+      <c r="G6" s="6">
+        <f>$E6*$F6</f>
+        <v/>
+      </c>
+      <c r="H6" s="15" t="n">
+        <v>200</v>
+      </c>
+      <c r="I6" s="6">
+        <f>TEXT($G6*$H6,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J6" s="6" t="inlineStr">
+        <is>
+          <t>Requirements Gathering</t>
+        </is>
+      </c>
+      <c r="K6" s="6" t="inlineStr">
+        <is>
+          <t>Deliverable: Azure architecture diagram with AI/ML service integration design</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="B7" s="7" t="inlineStr">
+        <is>
+          <t>Data Flow Design</t>
+        </is>
+      </c>
+      <c r="C7" s="7" t="inlineStr">
+        <is>
+          <t>Design document ingestion processing and output workflows</t>
+        </is>
+      </c>
+      <c r="D7" s="7" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E7" s="16" t="n">
+        <v>24</v>
+      </c>
+      <c r="F7" s="14">
+        <f>'Estimate Settings'!$C$25</f>
+        <v/>
+      </c>
+      <c r="G7" s="7">
+        <f>$E7*$F7</f>
+        <v/>
+      </c>
+      <c r="H7" s="17" t="n">
+        <v>180</v>
+      </c>
+      <c r="I7" s="7">
+        <f>TEXT($G7*$H7,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J7" s="7" t="inlineStr">
+        <is>
+          <t>Document Analysis</t>
+        </is>
+      </c>
+      <c r="K7" s="7" t="inlineStr">
+        <is>
+          <t>Deliverable: Document processing workflow and data flow diagrams</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="B8" s="6" t="inlineStr">
+        <is>
+          <t>Security Architecture</t>
+        </is>
+      </c>
+      <c r="C8" s="6" t="inlineStr">
+        <is>
+          <t>Design security controls encryption and access for documents</t>
+        </is>
+      </c>
+      <c r="D8" s="6" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E8" s="13" t="n">
+        <v>24</v>
+      </c>
+      <c r="F8" s="14">
+        <f>'Estimate Settings'!$C$25</f>
+        <v/>
+      </c>
+      <c r="G8" s="6">
+        <f>$E8*$F8</f>
+        <v/>
+      </c>
+      <c r="H8" s="15" t="n">
+        <v>175</v>
+      </c>
+      <c r="I8" s="6">
+        <f>TEXT($G8*$H8,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J8" s="6" t="inlineStr">
+        <is>
+          <t>Compliance Review</t>
+        </is>
+      </c>
+      <c r="K8" s="6" t="inlineStr">
+        <is>
+          <t>Document encryption at rest/transit RBAC roles and audit logging design</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>Planning</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>Project Planning</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="inlineStr">
+        <is>
+          <t>Develop implementation timeline and resource allocation</t>
+        </is>
+      </c>
+      <c r="D9" s="7" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E9" s="16" t="n">
+        <v>24</v>
+      </c>
+      <c r="F9" s="14">
+        <f>'Estimate Settings'!$C$25</f>
+        <v/>
+      </c>
+      <c r="G9" s="7">
+        <f>$E9*$F9</f>
+        <v/>
+      </c>
+      <c r="H9" s="17" t="n">
+        <v>140</v>
+      </c>
+      <c r="I9" s="7">
+        <f>TEXT($G9*$H9,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J9" s="7" t="inlineStr">
+        <is>
+          <t>IDP Solution Design</t>
+        </is>
+      </c>
+      <c r="K9" s="7" t="inlineStr">
+        <is>
+          <t>Deliverable: Project plan with phased rollout and milestone schedule</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>Development</t>
+        </is>
+      </c>
+      <c r="B10" s="6" t="inlineStr">
+        <is>
+          <t>Azure Infrastructure Setup</t>
+        </is>
+      </c>
+      <c r="C10" s="6" t="inlineStr">
+        <is>
+          <t>Provision Document Intelligence Cognitive Services Blob Storage and Functions</t>
+        </is>
+      </c>
+      <c r="D10" s="6" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E10" s="13" t="n">
+        <v>40</v>
+      </c>
+      <c r="F10" s="14">
+        <f>'Estimate Settings'!$C$26</f>
+        <v/>
+      </c>
+      <c r="G10" s="6">
+        <f>$E10*$F10</f>
+        <v/>
+      </c>
+      <c r="H10" s="15" t="n">
+        <v>160</v>
+      </c>
+      <c r="I10" s="6">
+        <f>TEXT($G10*$H10,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J10" s="6" t="inlineStr">
+        <is>
+          <t>IDP Solution Design</t>
+        </is>
+      </c>
+      <c r="K10" s="6" t="inlineStr">
+        <is>
+          <t>Includes Blob Storage containers Functions Logic Apps and Monitor setup</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>Development</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>Document Processing Pipeline</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="inlineStr">
+        <is>
+          <t>Build document ingestion and processing workflows</t>
+        </is>
+      </c>
+      <c r="D11" s="7" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E11" s="16" t="n">
+        <v>64</v>
+      </c>
+      <c r="F11" s="14">
+        <f>'Estimate Settings'!$C$26</f>
+        <v/>
+      </c>
+      <c r="G11" s="7">
+        <f>$E11*$F11</f>
+        <v/>
+      </c>
+      <c r="H11" s="17" t="n">
+        <v>130</v>
+      </c>
+      <c r="I11" s="7">
+        <f>TEXT($G11*$H11,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J11" s="7" t="inlineStr">
+        <is>
+          <t>Azure Infrastructure Setup</t>
+        </is>
+      </c>
+      <c r="K11" s="7" t="inlineStr">
+        <is>
+          <t>Serverless event-driven pipeline with error handling and retry logic</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>Development</t>
+        </is>
+      </c>
+      <c r="B12" s="6" t="inlineStr">
+        <is>
+          <t>AI/ML Model Integration</t>
+        </is>
+      </c>
+      <c r="C12" s="6" t="inlineStr">
+        <is>
+          <t>Integrate Azure Document Intelligence and Text Analytics services</t>
+        </is>
+      </c>
+      <c r="D12" s="6" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E12" s="13" t="n">
+        <v>48</v>
+      </c>
+      <c r="F12" s="14">
+        <f>'Estimate Settings'!$C$26</f>
+        <v/>
+      </c>
+      <c r="G12" s="6">
+        <f>$E12*$F12</f>
+        <v/>
+      </c>
+      <c r="H12" s="15" t="n">
+        <v>170</v>
+      </c>
+      <c r="I12" s="6">
+        <f>TEXT($G12*$H12,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J12" s="6" t="inlineStr">
+        <is>
+          <t>Document Processing Pipeline</t>
+        </is>
+      </c>
+      <c r="K12" s="6" t="inlineStr">
+        <is>
+          <t>Configure Document Intelligence APIs Text Analytics entity recognition workflows</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="inlineStr">
+        <is>
+          <t>Development</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>Custom Classification Models</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="inlineStr">
+        <is>
+          <t>Develop minimal classification logic for 2-3 document types</t>
+        </is>
+      </c>
+      <c r="D13" s="7" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E13" s="16" t="n">
+        <v>24</v>
+      </c>
+      <c r="F13" s="14">
+        <f>'Estimate Settings'!$C$26</f>
+        <v/>
+      </c>
+      <c r="G13" s="7">
+        <f>$E13*$F13</f>
+        <v/>
+      </c>
+      <c r="H13" s="17" t="n">
+        <v>165</v>
+      </c>
+      <c r="I13" s="7">
+        <f>TEXT($G13*$H13,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J13" s="7" t="inlineStr">
+        <is>
+          <t>AI/ML Model Integration</t>
+        </is>
+      </c>
+      <c r="K13" s="7" t="inlineStr">
+        <is>
+          <t>Simple classification using Azure pre-built services - not full custom ML models</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="inlineStr">
+        <is>
+          <t>Development</t>
+        </is>
+      </c>
+      <c r="B14" s="6" t="inlineStr">
+        <is>
+          <t>Data Extraction Logic</t>
+        </is>
+      </c>
+      <c r="C14" s="6" t="inlineStr">
+        <is>
+          <t>Build structured data extraction and validation logic</t>
+        </is>
+      </c>
+      <c r="D14" s="6" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E14" s="13" t="n">
+        <v>32</v>
+      </c>
+      <c r="F14" s="14">
+        <f>'Estimate Settings'!$C$26</f>
+        <v/>
+      </c>
+      <c r="G14" s="6">
+        <f>$E14*$F14</f>
+        <v/>
+      </c>
+      <c r="H14" s="15" t="n">
+        <v>130</v>
+      </c>
+      <c r="I14" s="6">
+        <f>TEXT($G14*$H14,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J14" s="6" t="inlineStr">
+        <is>
+          <t>Custom Classification Models</t>
+        </is>
+      </c>
+      <c r="K14" s="6" t="inlineStr">
+        <is>
+          <t>Includes field validation business rules and confidence scoring</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="inlineStr">
+        <is>
+          <t>Development</t>
+        </is>
+      </c>
+      <c r="B15" s="7" t="inlineStr">
+        <is>
+          <t>API Development</t>
+        </is>
+      </c>
+      <c r="C15" s="7" t="inlineStr">
+        <is>
+          <t>Create REST APIs for document submission and retrieval</t>
+        </is>
+      </c>
+      <c r="D15" s="7" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E15" s="16" t="n">
+        <v>24</v>
+      </c>
+      <c r="F15" s="14">
+        <f>'Estimate Settings'!$C$26</f>
+        <v/>
+      </c>
+      <c r="G15" s="7">
+        <f>$E15*$F15</f>
+        <v/>
+      </c>
+      <c r="H15" s="17" t="n">
+        <v>125</v>
+      </c>
+      <c r="I15" s="7">
+        <f>TEXT($G15*$H15,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J15" s="7" t="inlineStr">
+        <is>
+          <t>Data Extraction Logic</t>
+        </is>
+      </c>
+      <c r="K15" s="7" t="inlineStr">
+        <is>
+          <t>API Management endpoints with authentication and rate limiting</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="inlineStr">
+        <is>
+          <t>Development</t>
+        </is>
+      </c>
+      <c r="B16" s="6" t="inlineStr">
+        <is>
+          <t>Web Interface</t>
+        </is>
+      </c>
+      <c r="C16" s="6" t="inlineStr">
+        <is>
+          <t>Build document upload and results viewing interface</t>
+        </is>
+      </c>
+      <c r="D16" s="6" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E16" s="13" t="n">
+        <v>32</v>
+      </c>
+      <c r="F16" s="14">
+        <f>'Estimate Settings'!$C$26</f>
+        <v/>
+      </c>
+      <c r="G16" s="6">
+        <f>$E16*$F16</f>
+        <v/>
+      </c>
+      <c r="H16" s="15" t="n">
+        <v>125</v>
+      </c>
+      <c r="I16" s="6">
+        <f>TEXT($G16*$H16,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J16" s="6" t="inlineStr">
+        <is>
+          <t>API Development</t>
+        </is>
+      </c>
+      <c r="K16" s="6" t="inlineStr">
+        <is>
+          <t>Simple upload UI with drag-drop and results dashboard - not full application</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+      <c r="B17" s="7" t="inlineStr">
+        <is>
+          <t>Unit Testing</t>
+        </is>
+      </c>
+      <c r="C17" s="7" t="inlineStr">
+        <is>
+          <t>Develop automated tests for all processing components</t>
+        </is>
+      </c>
+      <c r="D17" s="7" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E17" s="16" t="n">
+        <v>32</v>
+      </c>
+      <c r="F17" s="14">
+        <f>'Estimate Settings'!$C$27</f>
+        <v/>
+      </c>
+      <c r="G17" s="7">
+        <f>$E17*$F17</f>
+        <v/>
+      </c>
+      <c r="H17" s="17" t="n">
+        <v>120</v>
+      </c>
+      <c r="I17" s="7">
+        <f>TEXT($G17*$H17,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J17" s="7" t="inlineStr">
+        <is>
+          <t>Data Extraction Logic</t>
+        </is>
+      </c>
+      <c r="K17" s="7" t="inlineStr">
+        <is>
+          <t>Automated test suite for Functions and API endpoints</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+      <c r="B18" s="6" t="inlineStr">
+        <is>
+          <t>Document Processing Testing</t>
+        </is>
+      </c>
+      <c r="C18" s="6" t="inlineStr">
+        <is>
+          <t>Test various document types formats and qualities</t>
+        </is>
+      </c>
+      <c r="D18" s="6" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E18" s="13" t="n">
+        <v>32</v>
+      </c>
+      <c r="F18" s="14">
+        <f>'Estimate Settings'!$C$27</f>
+        <v/>
+      </c>
+      <c r="G18" s="6">
+        <f>$E18*$F18</f>
+        <v/>
+      </c>
+      <c r="H18" s="15" t="n">
+        <v>120</v>
+      </c>
+      <c r="I18" s="6">
+        <f>TEXT($G18*$H18,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J18" s="6" t="inlineStr">
+        <is>
+          <t>Web Interface</t>
+        </is>
+      </c>
+      <c r="K18" s="6" t="inlineStr">
+        <is>
+          <t>Customer must provide comprehensive test document library with variations</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+      <c r="B19" s="7" t="inlineStr">
+        <is>
+          <t>Performance Testing</t>
+        </is>
+      </c>
+      <c r="C19" s="7" t="inlineStr">
+        <is>
+          <t>Test system performance with high document volumes</t>
+        </is>
+      </c>
+      <c r="D19" s="7" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E19" s="16" t="n">
+        <v>24</v>
+      </c>
+      <c r="F19" s="14">
+        <f>'Estimate Settings'!$C$27</f>
+        <v/>
+      </c>
+      <c r="G19" s="7">
+        <f>$E19*$F19</f>
+        <v/>
+      </c>
+      <c r="H19" s="17" t="n">
+        <v>140</v>
+      </c>
+      <c r="I19" s="7">
+        <f>TEXT($G19*$H19,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J19" s="7" t="inlineStr">
+        <is>
+          <t>Document Processing Testing</t>
+        </is>
+      </c>
+      <c r="K19" s="7" t="inlineStr">
+        <is>
+          <t>Load testing with realistic document volumes and concurrent processing</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+      <c r="B20" s="6" t="inlineStr">
+        <is>
+          <t>Accuracy Testing</t>
+        </is>
+      </c>
+      <c r="C20" s="6" t="inlineStr">
+        <is>
+          <t>Validate AI/ML model accuracy and data extraction quality</t>
+        </is>
+      </c>
+      <c r="D20" s="6" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E20" s="13" t="n">
+        <v>24</v>
+      </c>
+      <c r="F20" s="14">
+        <f>'Estimate Settings'!$C$27</f>
+        <v/>
+      </c>
+      <c r="G20" s="6">
+        <f>$E20*$F20</f>
+        <v/>
+      </c>
+      <c r="H20" s="15" t="n">
+        <v>170</v>
+      </c>
+      <c r="I20" s="6">
+        <f>TEXT($G20*$H20,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J20" s="6" t="inlineStr">
+        <is>
+          <t>Performance Testing</t>
+        </is>
+      </c>
+      <c r="K20" s="6" t="inlineStr">
+        <is>
+          <t>Statistical validation of extraction accuracy against labeled test dataset</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="7" t="inlineStr">
+        <is>
+          <t>Testing</t>
+        </is>
+      </c>
+      <c r="B21" s="7" t="inlineStr">
+        <is>
+          <t>Security Testing</t>
+        </is>
+      </c>
+      <c r="C21" s="7" t="inlineStr">
+        <is>
+          <t>Perform security testing on document handling pipeline</t>
+        </is>
+      </c>
+      <c r="D21" s="7" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E21" s="16" t="n">
+        <v>16</v>
+      </c>
+      <c r="F21" s="14">
+        <f>'Estimate Settings'!$C$27</f>
+        <v/>
+      </c>
+      <c r="G21" s="7">
+        <f>$E21*$F21</f>
+        <v/>
+      </c>
+      <c r="H21" s="17" t="n">
+        <v>175</v>
+      </c>
+      <c r="I21" s="7">
+        <f>TEXT($G21*$H21,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J21" s="7" t="inlineStr">
+        <is>
+          <t>Accuracy Testing</t>
+        </is>
+      </c>
+      <c r="K21" s="7" t="inlineStr">
+        <is>
+          <t>Includes RBAC policy validation encryption testing and audit log verification</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="inlineStr">
+        <is>
+          <t>Deployment</t>
+        </is>
+      </c>
+      <c r="B22" s="6" t="inlineStr">
+        <is>
+          <t>Production Deployment</t>
+        </is>
+      </c>
+      <c r="C22" s="6" t="inlineStr">
+        <is>
+          <t>Deploy IDP solution to production Azure environment</t>
+        </is>
+      </c>
+      <c r="D22" s="6" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E22" s="13" t="n">
+        <v>24</v>
+      </c>
+      <c r="F22" s="14">
+        <f>'Estimate Settings'!$C$28</f>
+        <v/>
+      </c>
+      <c r="G22" s="6">
+        <f>$E22*$F22</f>
+        <v/>
+      </c>
+      <c r="H22" s="15" t="n">
+        <v>160</v>
+      </c>
+      <c r="I22" s="6">
+        <f>TEXT($G22*$H22,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J22" s="6" t="inlineStr">
+        <is>
+          <t>Security Testing</t>
+        </is>
+      </c>
+      <c r="K22" s="6" t="inlineStr">
+        <is>
+          <t>Blue-green deployment with rollback procedures and smoke testing</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="7" t="inlineStr">
+        <is>
+          <t>Deployment</t>
+        </is>
+      </c>
+      <c r="B23" s="7" t="inlineStr">
+        <is>
+          <t>Model Deployment</t>
+        </is>
+      </c>
+      <c r="C23" s="7" t="inlineStr">
+        <is>
+          <t>Deploy trained ML models to production endpoints</t>
+        </is>
+      </c>
+      <c r="D23" s="7" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E23" s="16" t="n">
+        <v>16</v>
+      </c>
+      <c r="F23" s="14">
+        <f>'Estimate Settings'!$C$28</f>
+        <v/>
+      </c>
+      <c r="G23" s="7">
+        <f>$E23*$F23</f>
+        <v/>
+      </c>
+      <c r="H23" s="17" t="n">
+        <v>170</v>
+      </c>
+      <c r="I23" s="7">
+        <f>TEXT($G23*$H23,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J23" s="7" t="inlineStr">
+        <is>
+          <t>Production Deployment</t>
+        </is>
+      </c>
+      <c r="K23" s="7" t="inlineStr">
+        <is>
+          <t>Deploy classification logic and configure production Document Intelligence</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="inlineStr">
+        <is>
+          <t>Deployment</t>
+        </is>
+      </c>
+      <c r="B24" s="6" t="inlineStr">
+        <is>
+          <t>Go-Live Support</t>
+        </is>
+      </c>
+      <c r="C24" s="6" t="inlineStr">
+        <is>
+          <t>Provide support during initial production rollout</t>
+        </is>
+      </c>
+      <c r="D24" s="6" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E24" s="13" t="n">
+        <v>40</v>
+      </c>
+      <c r="F24" s="14">
+        <f>'Estimate Settings'!$C$28</f>
+        <v/>
+      </c>
+      <c r="G24" s="6">
+        <f>$E24*$F24</f>
+        <v/>
+      </c>
+      <c r="H24" s="15" t="n">
+        <v>110</v>
+      </c>
+      <c r="I24" s="6">
+        <f>TEXT($G24*$H24,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J24" s="6" t="inlineStr">
+        <is>
+          <t>Model Deployment</t>
+        </is>
+      </c>
+      <c r="K24" s="6" t="inlineStr">
+        <is>
+          <t>Daily monitoring rapid issue response and accuracy validation during hypercare</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="7" t="inlineStr">
+        <is>
+          <t>Training</t>
+        </is>
+      </c>
+      <c r="B25" s="7" t="inlineStr">
+        <is>
+          <t>Administrator Training</t>
+        </is>
+      </c>
+      <c r="C25" s="7" t="inlineStr">
+        <is>
+          <t>Train system administrators on IDP solution management</t>
+        </is>
+      </c>
+      <c r="D25" s="7" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E25" s="16" t="n">
+        <v>16</v>
+      </c>
+      <c r="F25" s="14">
+        <f>'Estimate Settings'!$C$29</f>
+        <v/>
+      </c>
+      <c r="G25" s="7">
+        <f>$E25*$F25</f>
+        <v/>
+      </c>
+      <c r="H25" s="17" t="n">
+        <v>130</v>
+      </c>
+      <c r="I25" s="7">
+        <f>TEXT($G25*$H25,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J25" s="7" t="inlineStr">
+        <is>
+          <t>Production Deployment</t>
+        </is>
+      </c>
+      <c r="K25" s="7" t="inlineStr">
+        <is>
+          <t>Includes Azure service management Monitor and troubleshooting</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="inlineStr">
+        <is>
+          <t>Training</t>
+        </is>
+      </c>
+      <c r="B26" s="6" t="inlineStr">
+        <is>
+          <t>Business User Training</t>
+        </is>
+      </c>
+      <c r="C26" s="6" t="inlineStr">
+        <is>
+          <t>Train users on document submission and results review</t>
+        </is>
+      </c>
+      <c r="D26" s="6" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E26" s="13" t="n">
+        <v>16</v>
+      </c>
+      <c r="F26" s="14">
+        <f>'Estimate Settings'!$C$29</f>
+        <v/>
+      </c>
+      <c r="G26" s="6">
+        <f>$E26*$F26</f>
+        <v/>
+      </c>
+      <c r="H26" s="15" t="n">
+        <v>120</v>
+      </c>
+      <c r="I26" s="6">
+        <f>TEXT($G26*$H26,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J26" s="6" t="inlineStr">
+        <is>
+          <t>Administrator Training</t>
+        </is>
+      </c>
+      <c r="K26" s="6" t="inlineStr">
+        <is>
+          <t>Role-based training for document processors and quality reviewers</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="7" t="inlineStr">
+        <is>
+          <t>Training</t>
+        </is>
+      </c>
+      <c r="B27" s="7" t="inlineStr">
+        <is>
+          <t>Documentation</t>
+        </is>
+      </c>
+      <c r="C27" s="7" t="inlineStr">
+        <is>
+          <t>Create user guides technical documentation and runbooks</t>
+        </is>
+      </c>
+      <c r="D27" s="7" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E27" s="16" t="n">
+        <v>24</v>
+      </c>
+      <c r="F27" s="14">
+        <f>'Estimate Settings'!$C$29</f>
+        <v/>
+      </c>
+      <c r="G27" s="7">
+        <f>$E27*$F27</f>
+        <v/>
+      </c>
+      <c r="H27" s="17" t="n">
+        <v>110</v>
+      </c>
+      <c r="I27" s="7">
+        <f>TEXT($G27*$H27,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J27" s="7" t="inlineStr">
+        <is>
+          <t>Business User Training</t>
+        </is>
+      </c>
+      <c r="K27" s="7" t="inlineStr">
+        <is>
+          <t>Deliverable: Operations runbook user guides and troubleshooting procedures</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="inlineStr">
+        <is>
+          <t>Closeout</t>
+        </is>
+      </c>
+      <c r="B28" s="6" t="inlineStr">
+        <is>
+          <t>Knowledge Transfer</t>
+        </is>
+      </c>
+      <c r="C28" s="6" t="inlineStr">
+        <is>
+          <t>Transfer solution ownership to client operations team</t>
+        </is>
+      </c>
+      <c r="D28" s="6" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E28" s="13" t="n">
+        <v>16</v>
+      </c>
+      <c r="F28" s="14">
+        <f>'Estimate Settings'!$C$30</f>
+        <v/>
+      </c>
+      <c r="G28" s="6">
+        <f>$E28*$F28</f>
+        <v/>
+      </c>
+      <c r="H28" s="15" t="n">
+        <v>140</v>
+      </c>
+      <c r="I28" s="6">
+        <f>TEXT($G28*$H28,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J28" s="6" t="inlineStr">
+        <is>
+          <t>Documentation</t>
+        </is>
+      </c>
+      <c r="K28" s="6" t="inlineStr">
+        <is>
+          <t>Comprehensive handover including Azure architecture model details and procedures</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="7" t="inlineStr">
+        <is>
+          <t>Closeout</t>
+        </is>
+      </c>
+      <c r="B29" s="7" t="inlineStr">
+        <is>
+          <t>Performance Baseline</t>
+        </is>
+      </c>
+      <c r="C29" s="7" t="inlineStr">
+        <is>
+          <t>Establish performance metrics and monitoring baselines</t>
+        </is>
+      </c>
+      <c r="D29" s="7" t="inlineStr">
+        <is>
+          <t>EO Engineer</t>
+        </is>
+      </c>
+      <c r="E29" s="16" t="n">
+        <v>8</v>
+      </c>
+      <c r="F29" s="14">
+        <f>'Estimate Settings'!$C$30</f>
+        <v/>
+      </c>
+      <c r="G29" s="7">
+        <f>$E29*$F29</f>
+        <v/>
+      </c>
+      <c r="H29" s="17" t="n">
+        <v>130</v>
+      </c>
+      <c r="I29" s="7">
+        <f>TEXT($G29*$H29,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J29" s="7" t="inlineStr">
+        <is>
+          <t>Knowledge Transfer</t>
+        </is>
+      </c>
+      <c r="K29" s="7" t="inlineStr">
+        <is>
+          <t>Establishes accuracy SLAs processing time metrics and cost monitoring</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="inlineStr">
+        <is>
+          <t>Management</t>
+        </is>
+      </c>
+      <c r="B30" s="6" t="inlineStr">
+        <is>
+          <t>Technical Leadership</t>
+        </is>
+      </c>
+      <c r="C30" s="6" t="inlineStr">
+        <is>
+          <t>Quarterback technical oversight and architecture review</t>
+        </is>
+      </c>
+      <c r="D30" s="6" t="inlineStr">
+        <is>
+          <t>EO Quarterback</t>
+        </is>
+      </c>
+      <c r="E30" s="6">
+        <f>ROUND(SUM($G$2:$G$29)*0.10,0)</f>
+        <v/>
+      </c>
+      <c r="F30" s="14">
+        <f>'Estimate Settings'!$C$32</f>
+        <v/>
+      </c>
+      <c r="G30" s="6">
+        <f>$E30*$F30</f>
+        <v/>
+      </c>
+      <c r="H30" s="15" t="n">
+        <v>200</v>
+      </c>
+      <c r="I30" s="6">
+        <f>TEXT($G30*$H30,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J30" s="6" t="inlineStr"/>
+      <c r="K30" s="6" t="inlineStr">
+        <is>
+          <t>Azure AI/ML architecture review and technical escalation support</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="7" t="inlineStr">
+        <is>
+          <t>Management</t>
+        </is>
+      </c>
+      <c r="B31" s="7" t="inlineStr">
+        <is>
+          <t>Project Management</t>
+        </is>
+      </c>
+      <c r="C31" s="7" t="inlineStr">
+        <is>
+          <t>Project coordination planning and management activities</t>
+        </is>
+      </c>
+      <c r="D31" s="7" t="inlineStr">
+        <is>
+          <t>EO Project Manager</t>
+        </is>
+      </c>
+      <c r="E31" s="7">
+        <f>ROUND(SUM($G$2:$G$29)*0.10,0)</f>
+        <v/>
+      </c>
+      <c r="F31" s="14">
+        <f>'Estimate Settings'!$C$31</f>
+        <v/>
+      </c>
+      <c r="G31" s="7">
+        <f>$E31*$F31</f>
+        <v/>
+      </c>
+      <c r="H31" s="17" t="n">
+        <v>150</v>
+      </c>
+      <c r="I31" s="7">
+        <f>TEXT($G31*$H31,"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J31" s="7" t="inlineStr"/>
+      <c r="K31" s="7" t="inlineStr">
+        <is>
+          <t>Includes weekly status reporting risk management and stakeholder coordination</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="6" t="inlineStr"/>
+      <c r="B32" s="6" t="inlineStr"/>
+      <c r="C32" s="6" t="inlineStr"/>
+      <c r="D32" s="6" t="inlineStr"/>
+      <c r="E32" s="13" t="inlineStr"/>
+      <c r="F32" s="14" t="inlineStr">
+        <is>
+          <t>TOTAL HOURS</t>
+        </is>
+      </c>
+      <c r="G32" s="6">
+        <f>SUM($G$2:$G$31)</f>
+        <v/>
+      </c>
+      <c r="H32" s="6" t="inlineStr">
+        <is>
+          <t>TOTAL COST</t>
+        </is>
+      </c>
+      <c r="I32" s="6">
+        <f>TEXT(SUMPRODUCT($G$2:$G$31,$H$2:$H$31),"$#,##0")</f>
+        <v/>
+      </c>
+      <c r="J32" s="6" t="inlineStr"/>
+      <c r="K32" s="6" t="inlineStr">
+        <is>
+          <t>EO Sales Engineer: Update phase-based multipliers in Estimate Settings based on customer document processing scope</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>